<commit_message>
Updated userinstructions + added about + added envdetails to plot panels loadtab
</commit_message>
<xml_diff>
--- a/templates/project-template.xlsx
+++ b/templates/project-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Koulu\Inssityö\Sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8640E913-11FF-46A0-BFB6-65294EE0F138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DA28A4-F310-465C-A5A3-7C981D35D117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7C859528-4B92-4A3E-BBEA-4268844455C3}"/>
+    <workbookView xWindow="4980" yWindow="5790" windowWidth="23295" windowHeight="9345" xr2:uid="{7C859528-4B92-4A3E-BBEA-4268844455C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Project-Example" sheetId="1" r:id="rId1"/>
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F528D44-B63F-41A3-A1DB-DECAF24AD9A1}">
   <dimension ref="A1:FN25"/>
   <sheetViews>
-    <sheetView topLeftCell="EM1" workbookViewId="0">
-      <selection activeCell="FB10" sqref="FB10"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="BK10" sqref="BK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,7 +1869,7 @@
         <v>99</v>
       </c>
       <c r="AM7" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AN7" s="5">
         <v>80</v>
@@ -1908,28 +1908,28 @@
         <v>100</v>
       </c>
       <c r="BJ7" s="5">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="EQ7" s="5">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="ER7" s="5">
-        <v>1</v>
+        <v>37.1</v>
       </c>
       <c r="ES7" s="5">
-        <v>2</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="ET7" s="5">
-        <v>3</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="EU7" s="5">
-        <v>4</v>
+        <v>37.4</v>
       </c>
       <c r="EV7" s="5">
-        <v>5</v>
+        <v>37.5</v>
       </c>
       <c r="FB7" s="5">
-        <v>10</v>
+        <v>38.1</v>
       </c>
     </row>
     <row r="8" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2012,7 +2012,7 @@
         <v>99</v>
       </c>
       <c r="AM8" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AN8" s="5">
         <v>80</v>
@@ -2057,31 +2057,31 @@
         <v>105</v>
       </c>
       <c r="BJ8" s="5">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="EQ8" s="5">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="ER8" s="5">
-        <v>1</v>
+        <v>37.1</v>
       </c>
       <c r="ES8" s="5">
-        <v>2</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="ET8" s="5">
-        <v>3</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="EU8" s="5">
-        <v>4</v>
+        <v>37.4</v>
       </c>
       <c r="EV8" s="5">
-        <v>5</v>
+        <v>37.5</v>
       </c>
       <c r="EW8" s="5">
-        <v>6</v>
+        <v>37.6</v>
       </c>
       <c r="FB8" s="5">
-        <v>11</v>
+        <v>38.200000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2173,7 +2173,7 @@
         <v>99</v>
       </c>
       <c r="AM9" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AN9" s="5">
         <v>80</v>
@@ -2224,34 +2224,34 @@
         <v>110</v>
       </c>
       <c r="BJ9" s="5">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="EQ9" s="5">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="ER9" s="5">
-        <v>1</v>
+        <v>37.1</v>
       </c>
       <c r="ES9" s="5">
-        <v>2</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="ET9" s="5">
-        <v>3</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="EU9" s="5">
-        <v>4</v>
+        <v>37.4</v>
       </c>
       <c r="EV9" s="5">
-        <v>5</v>
+        <v>37.5</v>
       </c>
       <c r="EW9" s="5">
-        <v>6</v>
+        <v>37.6</v>
       </c>
       <c r="EX9" s="5">
-        <v>7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="FB9" s="5">
-        <v>12</v>
+        <v>38.299999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:170" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2439,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D640ABA8-2FA5-4DE2-989F-A5A21C11C640}">
   <dimension ref="A1:FN25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EF1" workbookViewId="0">
-      <selection activeCell="EX12" sqref="EX12"/>
+    <sheetView topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BJ10" sqref="BJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,7 +3136,7 @@
         <v>99</v>
       </c>
       <c r="AM7" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AN7" s="5">
         <v>80</v>
@@ -3175,7 +3175,7 @@
         <v>100</v>
       </c>
       <c r="BJ7" s="5">
-        <v>105</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3258,7 +3258,7 @@
         <v>99</v>
       </c>
       <c r="AM8" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AN8" s="5">
         <v>80</v>
@@ -3303,7 +3303,7 @@
         <v>105</v>
       </c>
       <c r="BJ8" s="5">
-        <v>105</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3395,7 +3395,7 @@
         <v>99</v>
       </c>
       <c r="AM9" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AN9" s="5">
         <v>80</v>
@@ -3446,7 +3446,7 @@
         <v>110</v>
       </c>
       <c r="BJ9" s="5">
-        <v>115</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:170" s="3" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>